<commit_message>
Update root path for qualitron
</commit_message>
<xml_diff>
--- a/00_Master_database/Qualitron_Ruta.xlsx
+++ b/00_Master_database/Qualitron_Ruta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/13_Qualitron/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/13_Qualitron/00_Master_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{E2A4544D-DA94-46CF-8D14-EB2B8691097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79CD34F4-597A-4C9D-B425-A73424293285}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{E2A4544D-DA94-46CF-8D14-EB2B8691097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FD94F1-0F78-41EF-BDD1-D50FE983C897}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6223F5E1-400C-4BA4-9F78-0E04A4E01D04}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Ruta</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>Si</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
@@ -607,7 +604,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +855,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
@@ -879,7 +876,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Updated Main.py for sql export
</commit_message>
<xml_diff>
--- a/00_Master_database/Qualitron_Ruta.xlsx
+++ b/00_Master_database/Qualitron_Ruta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/13_Qualitron/00_Master_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{E2A4544D-DA94-46CF-8D14-EB2B8691097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1FD94F1-0F78-41EF-BDD1-D50FE983C897}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{E2A4544D-DA94-46CF-8D14-EB2B8691097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4C535D7-31D6-4F29-972D-2510ACC92D1E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6223F5E1-400C-4BA4-9F78-0E04A4E01D04}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{6223F5E1-400C-4BA4-9F78-0E04A4E01D04}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -604,7 +604,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the way to read the defects.
The code read a general defects and a specific defect
</commit_message>
<xml_diff>
--- a/00_Master_database/Qualitron_Ruta.xlsx
+++ b/00_Master_database/Qualitron_Ruta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/13_Qualitron/00_Master_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{E2A4544D-DA94-46CF-8D14-EB2B8691097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4C535D7-31D6-4F29-972D-2510ACC92D1E}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{E2A4544D-DA94-46CF-8D14-EB2B8691097E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62EB9E4A-F782-4924-BA22-44AECB8B958B}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{6223F5E1-400C-4BA4-9F78-0E04A4E01D04}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6223F5E1-400C-4BA4-9F78-0E04A4E01D04}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -604,15 +604,15 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A13"/>
+      <selection activeCell="A6" sqref="A6:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="7" width="23.5703125" customWidth="1"/>
+    <col min="6" max="7" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>58</v>
       </c>
@@ -635,7 +635,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>59</v>
       </c>
@@ -658,7 +658,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -681,7 +681,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
@@ -704,7 +704,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>59</v>
       </c>
@@ -727,7 +727,7 @@
         <v>1234567890</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>59</v>
       </c>
@@ -748,7 +748,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>59</v>
       </c>
@@ -769,7 +769,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>59</v>
       </c>
@@ -790,7 +790,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>59</v>
       </c>
@@ -811,7 +811,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>59</v>
       </c>
@@ -832,7 +832,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>59</v>
       </c>
@@ -853,7 +853,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -874,7 +874,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
@@ -895,7 +895,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -904,7 +904,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -913,7 +913,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -922,7 +922,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -931,7 +931,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -940,7 +940,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -949,7 +949,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -958,7 +958,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -967,7 +967,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>

</xml_diff>